<commit_message>
Started to implement lcd driver
</commit_message>
<xml_diff>
--- a/datasheet/Reverse Engineering/LCD bit mapping.xlsx
+++ b/datasheet/Reverse Engineering/LCD bit mapping.xlsx
@@ -389,32 +389,59 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -425,14 +452,14 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -443,15 +470,6 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -460,24 +478,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,6 +494,66 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>153521</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>127187</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>115421</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>127187</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="https://upload.wikimedia.org/wikipedia/commons/b/b2/14-segment.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7975227" y="4329393"/>
+          <a:ext cx="2449606" cy="4191000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -759,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AZ12"/>
+  <dimension ref="B2:AZ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W14" sqref="W14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,78 +881,78 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:52" x14ac:dyDescent="0.25">
-      <c r="AB2" s="36">
+      <c r="AB2" s="30">
         <v>7</v>
       </c>
-      <c r="AC2" s="37"/>
-      <c r="AD2" s="38"/>
-      <c r="AI2" s="36">
+      <c r="AC2" s="31"/>
+      <c r="AD2" s="32"/>
+      <c r="AI2" s="30">
         <v>19</v>
       </c>
-      <c r="AJ2" s="37"/>
-      <c r="AK2" s="38"/>
-      <c r="AM2" s="36">
+      <c r="AJ2" s="31"/>
+      <c r="AK2" s="32"/>
+      <c r="AM2" s="30">
         <v>31</v>
       </c>
-      <c r="AN2" s="37"/>
-      <c r="AO2" s="38"/>
+      <c r="AN2" s="31"/>
+      <c r="AO2" s="32"/>
     </row>
     <row r="3" spans="2:52" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="F3" s="9" t="s">
+      <c r="D3" s="23"/>
+      <c r="F3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="10"/>
-      <c r="K3" s="9" t="s">
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="23"/>
+      <c r="K3" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="10"/>
-      <c r="O3" s="9" t="s">
+      <c r="L3" s="23"/>
+      <c r="O3" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="P3" s="10"/>
-      <c r="R3" s="9" t="s">
+      <c r="P3" s="23"/>
+      <c r="R3" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="S3" s="13"/>
-      <c r="T3" s="10"/>
-      <c r="V3" s="9" t="s">
+      <c r="S3" s="22"/>
+      <c r="T3" s="23"/>
+      <c r="V3" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="W3" s="10"/>
+      <c r="W3" s="23"/>
       <c r="AA3" s="3"/>
-      <c r="AB3" s="27" t="s">
+      <c r="AB3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="AC3" s="28"/>
-      <c r="AD3" s="29"/>
+      <c r="AC3" s="25"/>
+      <c r="AD3" s="26"/>
       <c r="AE3" s="3"/>
-      <c r="AF3" s="27" t="s">
+      <c r="AF3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AG3" s="29"/>
+      <c r="AG3" s="26"/>
       <c r="AH3" s="3"/>
-      <c r="AI3" s="27" t="s">
+      <c r="AI3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="AJ3" s="28"/>
-      <c r="AK3" s="29"/>
+      <c r="AJ3" s="25"/>
+      <c r="AK3" s="26"/>
       <c r="AL3" s="3"/>
-      <c r="AM3" s="27" t="s">
+      <c r="AM3" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="AN3" s="28"/>
-      <c r="AO3" s="29"/>
+      <c r="AN3" s="25"/>
+      <c r="AO3" s="26"/>
       <c r="AP3" s="3"/>
-      <c r="AQ3" s="27" t="s">
+      <c r="AQ3" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="AR3" s="29"/>
+      <c r="AR3" s="26"/>
       <c r="AS3" s="3"/>
       <c r="AT3" s="3"/>
       <c r="AU3" s="3"/>
@@ -900,494 +960,488 @@
       <c r="AW3" s="3"/>
     </row>
     <row r="4" spans="2:52" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AQ4" s="23"/>
+      <c r="AQ4" s="15"/>
     </row>
     <row r="5" spans="2:52" s="2" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="10"/>
-      <c r="I5" s="9" t="s">
+      <c r="D5" s="22"/>
+      <c r="E5" s="23"/>
+      <c r="I5" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="10"/>
-      <c r="O5" s="9" t="s">
+      <c r="J5" s="22"/>
+      <c r="K5" s="23"/>
+      <c r="O5" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="10"/>
-      <c r="U5" s="27" t="s">
+      <c r="P5" s="22"/>
+      <c r="Q5" s="23"/>
+      <c r="U5" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="V5" s="28"/>
-      <c r="W5" s="29"/>
-      <c r="AC5" s="27" t="s">
+      <c r="V5" s="25"/>
+      <c r="W5" s="26"/>
+      <c r="AC5" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="AD5" s="28"/>
-      <c r="AE5" s="29"/>
-      <c r="AI5" s="18" t="s">
+      <c r="AD5" s="25"/>
+      <c r="AE5" s="26"/>
+      <c r="AI5" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="AJ5" s="19"/>
-      <c r="AK5" s="20"/>
-      <c r="AO5" s="18" t="s">
+      <c r="AJ5" s="28"/>
+      <c r="AK5" s="29"/>
+      <c r="AO5" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="AP5" s="19"/>
-      <c r="AQ5" s="20"/>
-      <c r="AU5" s="18" t="s">
+      <c r="AP5" s="28"/>
+      <c r="AQ5" s="29"/>
+      <c r="AU5" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="AV5" s="19"/>
-      <c r="AW5" s="20"/>
+      <c r="AV5" s="28"/>
+      <c r="AW5" s="29"/>
     </row>
     <row r="6" spans="2:52" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="N6" s="12" t="s">
+      <c r="N6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="O6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="P6" s="12" t="s">
+      <c r="P6" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="Q6" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="R6" s="12" t="s">
+      <c r="R6" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="T6" s="12" t="s">
+      <c r="T6" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="U6" s="11" t="s">
+      <c r="U6" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="V6" s="34" t="s">
+      <c r="V6" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="W6" s="33" t="s">
+      <c r="W6" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="X6" s="34" t="s">
+      <c r="X6" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="Z6" s="34" t="s">
+      <c r="Z6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="AB6" s="34" t="s">
+      <c r="AB6" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="AC6" s="35" t="s">
+      <c r="AC6" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="AD6" s="34" t="s">
+      <c r="AD6" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="AE6" s="33" t="s">
+      <c r="AE6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="AF6" s="15" t="s">
+      <c r="AF6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="AH6" s="15" t="s">
+      <c r="AH6" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="AI6" s="17" t="s">
+      <c r="AI6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="AJ6" s="15" t="s">
+      <c r="AJ6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="AK6" s="33" t="s">
+      <c r="AK6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="AL6" s="15" t="s">
+      <c r="AL6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AN6" s="15" t="s">
+      <c r="AN6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="AO6" s="17" t="s">
+      <c r="AO6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="AP6" s="15" t="s">
+      <c r="AP6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AQ6" s="33" t="s">
+      <c r="AQ6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="AR6" s="15" t="s">
+      <c r="AR6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="AT6" s="15" t="s">
+      <c r="AT6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="AU6" s="17" t="s">
+      <c r="AU6" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="AV6" s="15" t="s">
+      <c r="AV6" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="AW6" s="33" t="s">
+      <c r="AW6" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="AX6" s="34" t="s">
+      <c r="AX6" s="17" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:52" s="2" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="10" t="s">
         <v>7</v>
       </c>
       <c r="J7" s="3"/>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O7" s="12" t="s">
+      <c r="O7" s="10" t="s">
         <v>23</v>
       </c>
       <c r="P7" s="3"/>
-      <c r="Q7" s="12" t="s">
+      <c r="Q7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="U7" s="12" t="s">
+      <c r="U7" s="10" t="s">
         <v>49</v>
       </c>
       <c r="V7" s="3"/>
-      <c r="W7" s="34" t="s">
+      <c r="W7" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="AC7" s="34" t="s">
+      <c r="AC7" s="17" t="s">
         <v>45</v>
       </c>
       <c r="AD7" s="3"/>
-      <c r="AE7" s="34" t="s">
+      <c r="AE7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="AI7" s="15" t="s">
+      <c r="AI7" s="12" t="s">
         <v>30</v>
       </c>
       <c r="AJ7" s="3"/>
-      <c r="AK7" s="34" t="s">
+      <c r="AK7" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="AO7" s="15" t="s">
+      <c r="AO7" s="12" t="s">
         <v>7</v>
       </c>
       <c r="AP7" s="3"/>
-      <c r="AQ7" s="34" t="s">
+      <c r="AQ7" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="AU7" s="15" t="s">
+      <c r="AU7" s="12" t="s">
         <v>19</v>
       </c>
       <c r="AV7" s="3"/>
-      <c r="AW7" s="34" t="s">
+      <c r="AW7" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:52" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="12" t="s">
+      <c r="L8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="N8" s="12" t="s">
+      <c r="N8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="O8" s="14" t="s">
+      <c r="O8" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="P8" s="12" t="s">
+      <c r="P8" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="Q8" s="11" t="s">
+      <c r="Q8" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="R8" s="12" t="s">
+      <c r="R8" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="T8" s="12" t="s">
+      <c r="T8" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="U8" s="33" t="s">
+      <c r="U8" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="V8" s="34" t="s">
+      <c r="V8" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="W8" s="35" t="s">
+      <c r="W8" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="X8" s="34" t="s">
+      <c r="X8" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="Z8" s="34" t="s">
+      <c r="Z8" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="AB8" s="34" t="s">
+      <c r="AB8" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="AC8" s="33" t="s">
+      <c r="AC8" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AD8" s="34" t="s">
+      <c r="AD8" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="AE8" s="35" t="s">
+      <c r="AE8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="AF8" s="15" t="s">
+      <c r="AF8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="AH8" s="15" t="s">
+      <c r="AH8" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="AI8" s="16" t="s">
+      <c r="AI8" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="AJ8" s="15" t="s">
+      <c r="AJ8" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AK8" s="35" t="s">
+      <c r="AK8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="AL8" s="15" t="s">
+      <c r="AL8" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="AN8" s="15" t="s">
+      <c r="AN8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="AO8" s="16" t="s">
+      <c r="AO8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="AP8" s="15" t="s">
+      <c r="AP8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="AQ8" s="35" t="s">
+      <c r="AQ8" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="AR8" s="15" t="s">
+      <c r="AR8" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="AT8" s="15" t="s">
+      <c r="AT8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AU8" s="16" t="s">
+      <c r="AU8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="AV8" s="15" t="s">
+      <c r="AV8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="AW8" s="35" t="s">
+      <c r="AW8" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="AX8" s="34" t="s">
+      <c r="AX8" s="17" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="2:52" s="2" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="10"/>
-      <c r="I9" s="9" t="s">
+      <c r="D9" s="22"/>
+      <c r="E9" s="23"/>
+      <c r="I9" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="10"/>
-      <c r="O9" s="9" t="s">
+      <c r="J9" s="22"/>
+      <c r="K9" s="23"/>
+      <c r="O9" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="10"/>
-      <c r="U9" s="27" t="s">
+      <c r="P9" s="22"/>
+      <c r="Q9" s="23"/>
+      <c r="U9" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="V9" s="28"/>
-      <c r="W9" s="29"/>
-      <c r="Z9" s="34" t="s">
+      <c r="V9" s="25"/>
+      <c r="W9" s="26"/>
+      <c r="Z9" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="AC9" s="18" t="s">
+      <c r="AC9" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="AD9" s="19"/>
-      <c r="AE9" s="20"/>
-      <c r="AI9" s="18" t="s">
+      <c r="AD9" s="28"/>
+      <c r="AE9" s="29"/>
+      <c r="AI9" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="AJ9" s="19"/>
-      <c r="AK9" s="20"/>
-      <c r="AO9" s="18" t="s">
+      <c r="AJ9" s="28"/>
+      <c r="AK9" s="29"/>
+      <c r="AO9" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="AP9" s="19"/>
-      <c r="AQ9" s="20"/>
-      <c r="AU9" s="27" t="s">
+      <c r="AP9" s="28"/>
+      <c r="AQ9" s="29"/>
+      <c r="AU9" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AV9" s="28"/>
-      <c r="AW9" s="29"/>
+      <c r="AV9" s="25"/>
+      <c r="AW9" s="26"/>
     </row>
     <row r="10" spans="2:52" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="2:52" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="29"/>
-      <c r="F11" s="27" t="s">
+      <c r="D11" s="26"/>
+      <c r="F11" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="29"/>
-      <c r="K11" s="24" t="s">
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="26"/>
+      <c r="K11" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="27" t="s">
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="35"/>
+      <c r="O11" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="29"/>
-      <c r="AR11" s="21" t="s">
+      <c r="P11" s="25"/>
+      <c r="Q11" s="26"/>
+      <c r="AR11" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="AS11" s="21"/>
-      <c r="AT11" s="21"/>
-      <c r="AW11" s="22" t="s">
+      <c r="AS11" s="20"/>
+      <c r="AT11" s="20"/>
+      <c r="AW11" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AX11" s="22"/>
-      <c r="AY11" s="22"/>
-      <c r="AZ11" s="22"/>
+      <c r="AX11" s="19"/>
+      <c r="AY11" s="19"/>
+      <c r="AZ11" s="19"/>
     </row>
     <row r="12" spans="2:52" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K12" s="30" t="s">
+      <c r="K12" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="32"/>
-      <c r="O12" s="27" t="s">
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="29"/>
-      <c r="AC12" s="18" t="s">
+      <c r="P12" s="25"/>
+      <c r="Q12" s="26"/>
+      <c r="AC12" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="AD12" s="19"/>
-      <c r="AE12" s="19"/>
-      <c r="AF12" s="20"/>
-      <c r="AJ12" s="18" t="s">
+      <c r="AD12" s="28"/>
+      <c r="AE12" s="28"/>
+      <c r="AF12" s="29"/>
+      <c r="AJ12" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="AK12" s="20"/>
-      <c r="AN12" s="18" t="s">
+      <c r="AK12" s="29"/>
+      <c r="AN12" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="AO12" s="20"/>
-      <c r="AR12" s="21" t="s">
+      <c r="AO12" s="29"/>
+      <c r="AR12" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="AS12" s="21"/>
-      <c r="AT12" s="21"/>
-      <c r="AW12" s="22" t="s">
+      <c r="AS12" s="20"/>
+      <c r="AT12" s="20"/>
+      <c r="AW12" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="AX12" s="22"/>
-      <c r="AY12" s="22"/>
-      <c r="AZ12" s="22"/>
+      <c r="AX12" s="19"/>
+      <c r="AY12" s="19"/>
+      <c r="AZ12" s="19"/>
+    </row>
+    <row r="17" spans="27:27" x14ac:dyDescent="0.25">
+      <c r="AA17"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="AW11:AZ11"/>
-    <mergeCell ref="AW12:AZ12"/>
-    <mergeCell ref="AR11:AT11"/>
-    <mergeCell ref="AR12:AT12"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="U5:W5"/>
-    <mergeCell ref="U9:W9"/>
-    <mergeCell ref="AC5:AE5"/>
-    <mergeCell ref="AC9:AE9"/>
-    <mergeCell ref="AI5:AK5"/>
-    <mergeCell ref="AI9:AK9"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="R3:T3"/>
     <mergeCell ref="AU5:AW5"/>
     <mergeCell ref="AU9:AW9"/>
     <mergeCell ref="AB2:AD2"/>
@@ -1397,27 +1451,37 @@
     <mergeCell ref="AM2:AO2"/>
     <mergeCell ref="AM3:AO3"/>
     <mergeCell ref="AQ3:AR3"/>
+    <mergeCell ref="AO5:AQ5"/>
+    <mergeCell ref="AO9:AQ9"/>
+    <mergeCell ref="U5:W5"/>
+    <mergeCell ref="U9:W9"/>
+    <mergeCell ref="AC5:AE5"/>
+    <mergeCell ref="AC9:AE9"/>
+    <mergeCell ref="AI5:AK5"/>
+    <mergeCell ref="AI9:AK9"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="AW11:AZ11"/>
+    <mergeCell ref="AW12:AZ12"/>
+    <mergeCell ref="AR11:AT11"/>
+    <mergeCell ref="AR12:AT12"/>
+    <mergeCell ref="C9:E9"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="F11:I11"/>
     <mergeCell ref="O11:Q11"/>
     <mergeCell ref="O12:Q12"/>
     <mergeCell ref="K11:N11"/>
     <mergeCell ref="K12:N12"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="AO5:AQ5"/>
-    <mergeCell ref="AO9:AQ9"/>
     <mergeCell ref="AC12:AF12"/>
     <mergeCell ref="AJ12:AK12"/>
     <mergeCell ref="AN12:AO12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>